<commit_message>
Added sales analysis python script and sales analysis excel
</commit_message>
<xml_diff>
--- a/Amazon-Seller-Data-Analysis/sales_analysis.xlsx
+++ b/Amazon-Seller-Data-Analysis/sales_analysis.xlsx
@@ -32,12 +32,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF9999"/>
+        <bgColor rgb="00FF9999"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -58,11 +64,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -429,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,6 +455,16 @@
           <t>total_revenue</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MoM Growth (%)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Cumulative Sales</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -458,6 +475,10 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +489,10 @@
       <c r="B3" t="n">
         <v>0</v>
       </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -478,6 +503,10 @@
       <c r="B4" t="n">
         <v>1061.84</v>
       </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>1061.84</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -488,6 +517,12 @@
       <c r="B5" t="n">
         <v>10477.58</v>
       </c>
+      <c r="C5" t="n">
+        <v>886.74</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11539.42</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -498,6 +533,12 @@
       <c r="B6" t="n">
         <v>12671.12</v>
       </c>
+      <c r="C6" t="n">
+        <v>20.94</v>
+      </c>
+      <c r="D6" t="n">
+        <v>24210.54</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -508,6 +549,12 @@
       <c r="B7" t="n">
         <v>16112.24</v>
       </c>
+      <c r="C7" t="n">
+        <v>27.16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>40322.78</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -518,6 +565,12 @@
       <c r="B8" t="n">
         <v>32117.08</v>
       </c>
+      <c r="C8" t="n">
+        <v>99.33</v>
+      </c>
+      <c r="D8" t="n">
+        <v>72439.86</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -528,6 +581,12 @@
       <c r="B9" t="n">
         <v>8224.860000000001</v>
       </c>
+      <c r="C9" s="2" t="n">
+        <v>-74.39</v>
+      </c>
+      <c r="D9" t="n">
+        <v>80664.72</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -538,14 +597,26 @@
       <c r="B10" t="n">
         <v>8754.940000000001</v>
       </c>
+      <c r="C10" t="n">
+        <v>6.44</v>
+      </c>
+      <c r="D10" t="n">
+        <v>89419.66</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="3" t="n">
+        <v>89419.66</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>161.04</v>
+      </c>
+      <c r="D11" s="3" t="n">
         <v>89419.66</v>
       </c>
     </row>

</xml_diff>